<commit_message>
lecture 3 exercises done
</commit_message>
<xml_diff>
--- a/exercises/lecture 3/ch_P3ironsetsproduction_Answers.xlsx
+++ b/exercises/lecture 3/ch_P3ironsetsproduction_Answers.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392F01AB-760D-4402-8674-E66EFF0D407A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-28920" yWindow="3105" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operational Data" sheetId="1" r:id="rId1"/>
@@ -96,10 +97,23 @@
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="17" r:id="rId8"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -589,7 +603,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -719,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -734,36 +748,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
@@ -801,7 +810,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="41841.899535185185" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="60">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Author" refreshedDate="41841.899535185185" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E61" sheet="Operational Data"/>
   </cacheSource>
@@ -1267,7 +1276,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G1:J12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -1389,9 +1398,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1429,9 +1438,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1464,26 +1473,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1516,26 +1508,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1707,27 +1682,64 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="0" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{F19313F2-4D22-43B2-8916-23C18A30B42A}">
+  <we:reference id="wa200005271" version="2.5.5.0" store="fi-FI" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200005271" version="2.5.5.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_AI_TABLE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_FILL</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_ASK</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_FORMAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_EXTRACT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_TRANSLATE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_AI_CHOICE</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1743,7 +1755,7 @@
       <c r="E1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>116</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -1756,7 +1768,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1775,17 +1787,17 @@
       <c r="G2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="19">
         <v>3.0033333333333339</v>
       </c>
-      <c r="I2" s="23">
+      <c r="I2" s="20">
         <v>264.74666666666667</v>
       </c>
-      <c r="J2" s="22">
+      <c r="J2" s="19">
         <v>598.66666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1805,17 +1817,17 @@
       <c r="G3" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="19">
         <v>2.7850000000000001</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="20">
         <v>184.83666666666667</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="19">
         <v>626</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1835,17 +1847,17 @@
       <c r="G4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="19">
         <v>2.7566666666666664</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="20">
         <v>219.46833333333333</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="19">
         <v>635.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -1865,17 +1877,17 @@
       <c r="G5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="19">
         <v>2.9133333333333336</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="20">
         <v>221.32666666666668</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="19">
         <v>709.66666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -1895,17 +1907,17 @@
       <c r="G6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="19">
         <v>2.83</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="20">
         <v>211.14166666666665</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="19">
         <v>719.66666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -1925,17 +1937,17 @@
       <c r="G7" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="19">
         <v>2.8066666666666671</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="20">
         <v>198.11833333333334</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="19">
         <v>710.33333333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -1955,17 +1967,17 @@
       <c r="G8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="19">
         <v>2.9933333333333336</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="20">
         <v>190.84</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="19">
         <v>659.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -1985,17 +1997,17 @@
       <c r="G9" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="19">
         <v>2.83</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="20">
         <v>202.17</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="19">
         <v>784.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -2015,17 +2027,17 @@
       <c r="G10" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="19">
         <v>2.8650000000000002</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="20">
         <v>173.76333333333332</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="19">
         <v>676.83333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -2045,17 +2057,17 @@
       <c r="G11" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="19">
         <v>2.8266666666666667</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="20">
         <v>250.34166666666667</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="19">
         <v>761.33333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -2074,17 +2086,17 @@
       <c r="G12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="19">
         <v>2.8610000000000011</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="19">
         <v>211.67533333333333</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="19">
         <v>688.2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -2102,7 +2114,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -2120,7 +2132,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -2156,7 +2168,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -2192,7 +2204,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -2210,7 +2222,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>107</v>
       </c>
@@ -2228,7 +2240,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -2246,7 +2258,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -2263,7 +2275,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -2281,7 +2293,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -2299,7 +2311,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -2317,7 +2329,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -2335,7 +2347,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -2353,7 +2365,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -2371,7 +2383,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -2389,7 +2401,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -2407,7 +2419,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>108</v>
       </c>
@@ -2425,7 +2437,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -2442,7 +2454,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -2460,7 +2472,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2496,7 +2508,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -2532,7 +2544,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2550,7 +2562,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>106</v>
       </c>
@@ -2568,7 +2580,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -2586,7 +2598,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -2604,7 +2616,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -2621,7 +2633,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -2639,7 +2651,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -2657,7 +2669,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>103</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>104</v>
       </c>
@@ -2693,7 +2705,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -2711,7 +2723,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2729,7 +2741,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -2747,7 +2759,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -2765,7 +2777,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -2783,7 +2795,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2818,7 +2830,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -2836,7 +2848,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2854,7 +2866,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2872,7 +2884,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>99</v>
       </c>
@@ -2890,7 +2902,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>105</v>
       </c>
@@ -2908,7 +2920,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>107</v>
       </c>
@@ -2944,7 +2956,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>108</v>
       </c>
@@ -2969,947 +2981,947 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>5638.7466999999997</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>4556204.5506999996</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="15">
         <v>1</v>
       </c>
-      <c r="E21" s="18">
-        <v>500</v>
-      </c>
-      <c r="F21" s="16" t="s">
+      <c r="E21" s="15">
+        <v>500</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="15">
         <v>1</v>
       </c>
-      <c r="E22" s="18">
-        <v>500</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="E22" s="15">
+        <v>500</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="15">
         <v>1</v>
       </c>
-      <c r="E23" s="18">
-        <v>500</v>
-      </c>
-      <c r="F23" s="16" t="s">
+      <c r="E23" s="15">
+        <v>500</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="15">
         <v>1</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="15">
         <v>1000</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="15">
         <v>1</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="15">
         <v>1000</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="15">
         <v>1</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="15">
         <v>972.68408551068762</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="15">
         <v>1</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="15">
         <v>1000</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="15">
         <v>1</v>
       </c>
-      <c r="E28" s="18">
-        <v>500</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="E28" s="15">
+        <v>500</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="15">
         <v>1</v>
       </c>
-      <c r="E29" s="18">
-        <v>500</v>
-      </c>
-      <c r="F29" s="16" t="s">
+      <c r="E29" s="15">
+        <v>500</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="14">
         <v>1</v>
       </c>
-      <c r="E30" s="19">
-        <v>500</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="E30" s="14">
+        <v>500</v>
+      </c>
+      <c r="F30" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="25" t="s">
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="F34" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G34" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="16" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="17">
         <v>315.11</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="16">
+      <c r="G35" s="15">
         <v>19684.89</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="16" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D36" s="17">
         <v>403.75333333333333</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G36" s="16">
+      <c r="G36" s="15">
         <v>19596.246666666666</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="17">
         <v>470.255</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="15">
         <v>19529.744999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="16" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="17">
         <v>862.13</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G38" s="16">
+      <c r="G38" s="15">
         <v>19137.87</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="16" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D39" s="17">
         <v>875.64833333333331</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G39" s="16">
+      <c r="G39" s="15">
         <v>19124.351666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="16" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="20">
+      <c r="D40" s="17">
         <v>789.60500000000002</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G40" s="15">
         <v>19210.395</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="16" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="20">
+      <c r="D41" s="17">
         <v>989.41666666666663</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="15">
         <v>19010.583333333332</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="16" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="17">
         <v>484.62</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G42" s="16">
+      <c r="G42" s="15">
         <v>19515.38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D43" s="20">
+      <c r="D43" s="17">
         <v>211.62666666666667</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="15">
         <v>19788.373333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="16" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D44" s="20">
+      <c r="D44" s="17">
         <v>236.58166666666671</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G44" s="15">
         <v>19763.418333333335</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="16" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="17">
         <v>19999.999999999996</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="16" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D46" s="18">
-        <v>500</v>
-      </c>
-      <c r="E46" s="16" t="s">
+      <c r="D46" s="15">
+        <v>500</v>
+      </c>
+      <c r="E46" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G46" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="G46" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="18">
-        <v>500</v>
-      </c>
-      <c r="E47" s="16" t="s">
+      <c r="D47" s="15">
+        <v>500</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="F47" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G47" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
+      <c r="G47" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D48" s="18">
-        <v>500</v>
-      </c>
-      <c r="E48" s="16" t="s">
+      <c r="D48" s="15">
+        <v>500</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F48" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G48" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="16" t="s">
+      <c r="G48" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D49" s="18">
+      <c r="D49" s="15">
         <v>1000</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="16" t="s">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="18">
+      <c r="D50" s="15">
         <v>1000</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="16" t="s">
+      <c r="F50" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="16">
+      <c r="G50" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="16" t="s">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D51" s="18">
+      <c r="D51" s="15">
         <v>972.68408551068762</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G51" s="16">
+      <c r="G51" s="15">
         <v>27.315914489312377</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="16" t="s">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D52" s="18">
+      <c r="D52" s="15">
         <v>1000</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="F52" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G52" s="16">
+      <c r="G52" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="16" t="s">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D53" s="18">
-        <v>500</v>
-      </c>
-      <c r="E53" s="16" t="s">
+      <c r="D53" s="15">
+        <v>500</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F53" s="16" t="s">
+      <c r="F53" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G53" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="16" t="s">
+      <c r="G53" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D54" s="18">
-        <v>500</v>
-      </c>
-      <c r="E54" s="16" t="s">
+      <c r="D54" s="15">
+        <v>500</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F54" s="16" t="s">
+      <c r="F54" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G54" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="16" t="s">
+      <c r="G54" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="18">
-        <v>500</v>
-      </c>
-      <c r="E55" s="16" t="s">
+      <c r="D55" s="15">
+        <v>500</v>
+      </c>
+      <c r="E55" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="F55" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G55" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="16" t="s">
+      <c r="G55" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="18">
-        <v>500</v>
-      </c>
-      <c r="E56" s="16" t="s">
+      <c r="D56" s="15">
+        <v>500</v>
+      </c>
+      <c r="E56" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="F56" s="16" t="s">
+      <c r="F56" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G56" s="18">
+      <c r="G56" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="16" t="s">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D57" s="18">
-        <v>500</v>
-      </c>
-      <c r="E57" s="16" t="s">
+      <c r="D57" s="15">
+        <v>500</v>
+      </c>
+      <c r="E57" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="F57" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G57" s="18">
+      <c r="G57" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="16" t="s">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="18">
-        <v>500</v>
-      </c>
-      <c r="E58" s="16" t="s">
+      <c r="D58" s="15">
+        <v>500</v>
+      </c>
+      <c r="E58" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F58" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G58" s="18">
+      <c r="G58" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="16" t="s">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D59" s="18">
+      <c r="D59" s="15">
         <v>1000</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F59" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G59" s="18">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="16" t="s">
+      <c r="G59" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="18">
+      <c r="D60" s="15">
         <v>1000</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G60" s="18">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="16" t="s">
+      <c r="G60" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D61" s="18">
+      <c r="D61" s="15">
         <v>972.68408551068762</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="F61" s="16" t="s">
+      <c r="F61" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="18">
+      <c r="G61" s="15">
         <v>472.68408551068762</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="16" t="s">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D62" s="15">
         <v>1000</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G62" s="18">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="16" t="s">
+      <c r="G62" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D63" s="18">
-        <v>500</v>
-      </c>
-      <c r="E63" s="16" t="s">
+      <c r="D63" s="15">
+        <v>500</v>
+      </c>
+      <c r="E63" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="F63" s="16" t="s">
+      <c r="F63" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G63" s="18">
+      <c r="G63" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="16" t="s">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="18">
-        <v>500</v>
-      </c>
-      <c r="E64" s="16" t="s">
+      <c r="D64" s="15">
+        <v>500</v>
+      </c>
+      <c r="E64" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="F64" s="16" t="s">
+      <c r="F64" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G64" s="18">
+      <c r="G64" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="15" t="s">
+    <row r="65" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D65" s="19">
-        <v>500</v>
-      </c>
-      <c r="E65" s="15" t="s">
+      <c r="D65" s="14">
+        <v>500</v>
+      </c>
+      <c r="E65" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="F65" s="15" t="s">
+      <c r="F65" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G65" s="19">
+      <c r="G65" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3920,610 +3932,610 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="16">
-        <v>500</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="D9" s="15">
+        <v>500</v>
+      </c>
+      <c r="E9" s="15">
         <v>-529.82361638954842</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>315.11</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>529.82361638954842</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="16">
-        <v>500</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="D10" s="15">
+        <v>500</v>
+      </c>
+      <c r="E10" s="15">
         <v>-379.75614113222446</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <v>403.75333333333333</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="15">
         <v>379.75614113222446</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="16">
-        <v>500</v>
-      </c>
-      <c r="E11" s="16">
+      <c r="D11" s="15">
+        <v>500</v>
+      </c>
+      <c r="E11" s="15">
         <v>-305.28340261282597</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <v>470.255</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <v>305.28340261282597</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>1000</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>42.516258907363749</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <v>862.13000000000011</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <v>42.516258907363749</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>1000</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <v>79.478921219319204</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="15">
         <v>875.64833333333308</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <v>79.478921219319204</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="15">
         <v>972.68408551068762</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="15">
         <v>0</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="15">
         <v>789.60500000000002</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="15">
         <v>40.959599542334423</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <v>308.98068904593657</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <v>1000</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <v>147.29636975455321</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <v>989.41666666666652</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>147.29636975455321</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="16">
-        <v>500</v>
-      </c>
-      <c r="E16" s="16">
+      <c r="D16" s="15">
+        <v>500</v>
+      </c>
+      <c r="E16" s="15">
         <v>-311.54941211401444</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <v>484.61999999999989</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="15">
         <v>311.54941211401444</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="16">
-        <v>500</v>
-      </c>
-      <c r="E17" s="16">
+      <c r="D17" s="15">
+        <v>500</v>
+      </c>
+      <c r="E17" s="15">
         <v>-594.38936361836886</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="15">
         <v>211.62666666666701</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="15">
         <v>594.38936361836886</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="15">
-        <v>500</v>
-      </c>
-      <c r="E18" s="15">
+      <c r="D18" s="14">
+        <v>500</v>
+      </c>
+      <c r="E18" s="14">
         <v>-558.64997228820232</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>236.58166666666693</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="14">
         <v>558.64997228820232</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="27" t="s">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="15">
         <v>315.11</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="15">
         <v>0</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="15">
         <v>20000</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G23" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="15">
         <v>19684.89</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="15">
         <v>403.75333333333333</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="15">
         <v>0</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="15">
         <v>20000</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="15">
         <v>19596.246666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <v>470.255</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="15">
         <v>0</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="15">
         <v>20000</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="15">
         <v>19529.744999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <v>862.13</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="15">
         <v>0</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="15">
         <v>20000</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="15">
         <v>19137.87</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="15">
         <v>875.64833333333331</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="15">
         <v>0</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="15">
         <v>20000</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="15">
         <v>19124.351666666666</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="15">
         <v>789.60500000000002</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="15">
         <v>0</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <v>20000</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="15">
         <v>19210.395</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="15">
         <v>989.41666666666663</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="15">
         <v>0</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="15">
         <v>20000</v>
       </c>
-      <c r="G29" s="16">
+      <c r="G29" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="15">
         <v>19010.583333333332</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="15">
         <v>484.62</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="15">
         <v>0</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="15">
         <v>20000</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="15">
         <v>19515.38</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="15">
         <v>211.62666666666667</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="15">
         <v>0</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="15">
         <v>20000</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G31" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="15">
         <v>19788.373333333333</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="15">
         <v>236.58166666666671</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="15">
         <v>0</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="15">
         <v>20000</v>
       </c>
-      <c r="G32" s="16">
+      <c r="G32" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H32" s="16">
+      <c r="H32" s="15">
         <v>19763.418333333335</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15" t="s">
+    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="14">
         <v>19999.999999999996</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="14">
         <v>281.33194774346777</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="14">
         <v>20000</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="14">
         <v>76.66666666667011</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <v>1326.666666666664</v>
       </c>
     </row>
@@ -4534,340 +4546,340 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26" t="s">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="26"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="24" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>4556204.5506999996</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="26" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="F11" s="26" t="s">
+      <c r="D11" s="23"/>
+      <c r="F11" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="18">
-        <v>500</v>
-      </c>
-      <c r="F13" s="18">
-        <v>500</v>
-      </c>
-      <c r="G13" s="18">
+      <c r="D13" s="15">
+        <v>500</v>
+      </c>
+      <c r="F13" s="15">
+        <v>500</v>
+      </c>
+      <c r="G13" s="15">
         <v>4556204.55</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="15">
         <v>499.99999999988853</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="18">
-        <v>500</v>
-      </c>
-      <c r="F14" s="18">
-        <v>500</v>
-      </c>
-      <c r="G14" s="18">
+      <c r="D14" s="15">
+        <v>500</v>
+      </c>
+      <c r="F14" s="15">
+        <v>500</v>
+      </c>
+      <c r="G14" s="15">
         <v>4556204.55</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="15">
         <v>500.00000000002746</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="18">
-        <v>500</v>
-      </c>
-      <c r="F15" s="18">
-        <v>500</v>
-      </c>
-      <c r="G15" s="18">
+      <c r="D15" s="15">
+        <v>500</v>
+      </c>
+      <c r="F15" s="15">
+        <v>500</v>
+      </c>
+      <c r="G15" s="15">
         <v>4556204.55</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="15">
         <v>499.99999999975586</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="15">
         <v>1000</v>
       </c>
-      <c r="F16" s="18">
-        <v>500</v>
-      </c>
-      <c r="G16" s="18">
+      <c r="F16" s="15">
+        <v>500</v>
+      </c>
+      <c r="G16" s="15">
         <v>4125139.55</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="15">
         <v>999.99999999981765</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>1000</v>
       </c>
-      <c r="F17" s="18">
-        <v>500</v>
-      </c>
-      <c r="G17" s="18">
+      <c r="F17" s="15">
+        <v>500</v>
+      </c>
+      <c r="G17" s="15">
         <v>4118380.38</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="15">
         <v>999.99999999938427</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="15">
         <v>972.68408551068762</v>
       </c>
-      <c r="F18" s="18">
-        <v>500</v>
-      </c>
-      <c r="G18" s="18">
+      <c r="F18" s="15">
+        <v>500</v>
+      </c>
+      <c r="G18" s="15">
         <v>4182970.83</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="15">
         <v>972.68408551047037</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="15">
         <v>1000</v>
       </c>
-      <c r="F19" s="18">
-        <v>500</v>
-      </c>
-      <c r="G19" s="18">
+      <c r="F19" s="15">
+        <v>500</v>
+      </c>
+      <c r="G19" s="15">
         <v>4061496.22</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="15">
         <v>1000</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="18">
-        <v>500</v>
-      </c>
-      <c r="F20" s="18">
-        <v>500</v>
-      </c>
-      <c r="G20" s="18">
+      <c r="D20" s="15">
+        <v>500</v>
+      </c>
+      <c r="F20" s="15">
+        <v>500</v>
+      </c>
+      <c r="G20" s="15">
         <v>4556204.55</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="15">
         <v>499.99999999969276</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="18">
-        <v>500</v>
-      </c>
-      <c r="F21" s="18">
-        <v>500</v>
-      </c>
-      <c r="G21" s="18">
+      <c r="D21" s="15">
+        <v>500</v>
+      </c>
+      <c r="F21" s="15">
+        <v>500</v>
+      </c>
+      <c r="G21" s="15">
         <v>4556204.55</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="15">
         <v>499.99999999972192</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="15">
         <v>4556204.55</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="19">
-        <v>500</v>
-      </c>
-      <c r="F22" s="19">
-        <v>500</v>
-      </c>
-      <c r="G22" s="19">
+      <c r="D22" s="14">
+        <v>500</v>
+      </c>
+      <c r="F22" s="14">
+        <v>500</v>
+      </c>
+      <c r="G22" s="14">
         <v>4556204.55</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="14">
         <v>499.99999999981208</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J22" s="14">
         <v>4556204.55</v>
       </c>
     </row>
@@ -4878,28 +4890,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4921,25 +4933,25 @@
       <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'Operational Data'!G2</f>
         <v>C Forged Irons</v>
@@ -4955,10 +4967,10 @@
         <f>'Operational Data'!I2</f>
         <v>264.74666666666667</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="18">
         <v>699.99</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f>E2-(D2+C2*40)</f>
         <v>315.11</v>
       </c>
@@ -4966,13 +4978,13 @@
         <f>'Operational Data'!J2</f>
         <v>598.66666666666663</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="21">
         <v>1000</v>
       </c>
-      <c r="I2" s="13">
-        <v>500</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="I2" s="12">
+        <v>500</v>
+      </c>
+      <c r="J2" s="13">
         <f>SUMPRODUCT(F2:F11,I2:I11)</f>
         <v>4556204.5506729987</v>
       </c>
@@ -4984,7 +4996,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'Operational Data'!G3</f>
         <v>Clean Pro Irons</v>
@@ -5000,10 +5012,10 @@
         <f>'Operational Data'!I3</f>
         <v>184.83666666666667</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="18">
         <v>699.99</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f t="shared" ref="F3:F11" si="0">E3-(D3+C3*40)</f>
         <v>403.75333333333333</v>
       </c>
@@ -5011,14 +5023,14 @@
         <f>'Operational Data'!J3</f>
         <v>626</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="21">
         <v>1000</v>
       </c>
-      <c r="I3" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I3" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>'Operational Data'!G4</f>
         <v>Clean Shot Irons</v>
@@ -5034,10 +5046,10 @@
         <f>'Operational Data'!I4</f>
         <v>219.46833333333333</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="18">
         <v>799.99</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f t="shared" si="0"/>
         <v>470.255</v>
       </c>
@@ -5045,14 +5057,14 @@
         <f>'Operational Data'!J4</f>
         <v>635.5</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="21">
         <v>1000</v>
       </c>
-      <c r="I4" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I4" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>'Operational Data'!G5</f>
         <v>Hybrid Set</v>
@@ -5068,10 +5080,10 @@
         <f>'Operational Data'!I5</f>
         <v>221.32666666666668</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="18">
         <v>1199.99</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>862.13</v>
       </c>
@@ -5079,14 +5091,14 @@
         <f>'Operational Data'!J5</f>
         <v>709.66666666666663</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="21">
         <v>1000</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>'Operational Data'!G6</f>
         <v>Hybrids/Irons Combo Set</v>
@@ -5102,10 +5114,10 @@
         <f>'Operational Data'!I6</f>
         <v>211.14166666666665</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="18">
         <v>1199.99</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>875.64833333333331</v>
       </c>
@@ -5113,14 +5125,14 @@
         <f>'Operational Data'!J6</f>
         <v>719.66666666666663</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>1000</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>'Operational Data'!G7</f>
         <v>Pro Irons</v>
@@ -5136,10 +5148,10 @@
         <f>'Operational Data'!I7</f>
         <v>198.11833333333334</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>1099.99</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>789.60500000000002</v>
       </c>
@@ -5147,14 +5159,14 @@
         <f>'Operational Data'!J7</f>
         <v>710.33333333333337</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <v>1000</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>972.68408551068762</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>'Operational Data'!G8</f>
         <v>Pro Irons/Hybrids Combo Set</v>
@@ -5170,10 +5182,10 @@
         <f>'Operational Data'!I8</f>
         <v>190.84</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="18">
         <v>1299.99</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="0"/>
         <v>989.41666666666663</v>
       </c>
@@ -5181,14 +5193,14 @@
         <f>'Operational Data'!J8</f>
         <v>659.5</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="21">
         <v>1000</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>'Operational Data'!G9</f>
         <v>Prototype Irons</v>
@@ -5204,10 +5216,10 @@
         <f>'Operational Data'!I9</f>
         <v>202.17</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>799.99</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f t="shared" si="0"/>
         <v>484.62</v>
       </c>
@@ -5215,14 +5227,14 @@
         <f>'Operational Data'!J9</f>
         <v>784.5</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <v>1000</v>
       </c>
-      <c r="I9" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I9" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>'Operational Data'!G10</f>
         <v>Standard Irons</v>
@@ -5238,10 +5250,10 @@
         <f>'Operational Data'!I10</f>
         <v>173.76333333333332</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>499.99</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>211.62666666666667</v>
       </c>
@@ -5249,14 +5261,14 @@
         <f>'Operational Data'!J10</f>
         <v>676.83333333333337</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>1000</v>
       </c>
-      <c r="I10" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I10" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>'Operational Data'!G11</f>
         <v>X Forged Irons</v>
@@ -5272,10 +5284,10 @@
         <f>'Operational Data'!I11</f>
         <v>250.34166666666667</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="18">
         <v>599.99</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>236.58166666666671</v>
       </c>
@@ -5283,67 +5295,67 @@
         <f>'Operational Data'!J11</f>
         <v>761.33333333333337</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="21">
         <v>1000</v>
       </c>
-      <c r="I11" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="22"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="22"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="22"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="22"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="22"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="22"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="22"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="I11" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="18"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="18"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5352,28 +5364,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5395,25 +5407,25 @@
       <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'Operational Data'!G2</f>
         <v>C Forged Irons</v>
@@ -5429,10 +5441,10 @@
         <f>'Operational Data'!I2</f>
         <v>264.74666666666667</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="18">
         <v>699.99</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f>E2-(D2+C2*40)</f>
         <v>315.11</v>
       </c>
@@ -5440,13 +5452,13 @@
         <f>'Operational Data'!J2</f>
         <v>598.66666666666663</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="21">
         <v>1000</v>
       </c>
-      <c r="I2" s="13">
-        <v>500</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="I2" s="12">
+        <v>500</v>
+      </c>
+      <c r="J2" s="13">
         <f>SUMPRODUCT(D2:D11,I2:I11)</f>
         <v>1430038.1789390335</v>
       </c>
@@ -5458,7 +5470,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'Operational Data'!G3</f>
         <v>Clean Pro Irons</v>
@@ -5474,10 +5486,10 @@
         <f>'Operational Data'!I3</f>
         <v>184.83666666666667</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="18">
         <v>699.99</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f t="shared" ref="F3:F11" si="0">E3-(D3+C3*40)</f>
         <v>403.75333333333333</v>
       </c>
@@ -5485,14 +5497,14 @@
         <f>'Operational Data'!J3</f>
         <v>626</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="21">
         <v>1000</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>'Operational Data'!G4</f>
         <v>Clean Shot Irons</v>
@@ -5508,10 +5520,10 @@
         <f>'Operational Data'!I4</f>
         <v>219.46833333333333</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="18">
         <v>799.99</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f t="shared" si="0"/>
         <v>470.255</v>
       </c>
@@ -5519,14 +5531,14 @@
         <f>'Operational Data'!J4</f>
         <v>635.5</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="21">
         <v>1000</v>
       </c>
-      <c r="I4" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I4" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>'Operational Data'!G5</f>
         <v>Hybrid Set</v>
@@ -5542,10 +5554,10 @@
         <f>'Operational Data'!I5</f>
         <v>221.32666666666668</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="18">
         <v>1199.99</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>862.13</v>
       </c>
@@ -5553,14 +5565,14 @@
         <f>'Operational Data'!J5</f>
         <v>709.66666666666663</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="21">
         <v>1000</v>
       </c>
-      <c r="I5" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I5" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>'Operational Data'!G6</f>
         <v>Hybrids/Irons Combo Set</v>
@@ -5576,10 +5588,10 @@
         <f>'Operational Data'!I6</f>
         <v>211.14166666666665</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="18">
         <v>1199.99</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>875.64833333333331</v>
       </c>
@@ -5587,14 +5599,14 @@
         <f>'Operational Data'!J6</f>
         <v>719.66666666666663</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>1000</v>
       </c>
-      <c r="I6" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>'Operational Data'!G7</f>
         <v>Pro Irons</v>
@@ -5610,10 +5622,10 @@
         <f>'Operational Data'!I7</f>
         <v>198.11833333333334</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>1099.99</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>789.60500000000002</v>
       </c>
@@ -5621,14 +5633,14 @@
         <f>'Operational Data'!J7</f>
         <v>710.33333333333337</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <v>1000</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>989.31116389548527</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>'Operational Data'!G8</f>
         <v>Pro Irons/Hybrids Combo Set</v>
@@ -5644,10 +5656,10 @@
         <f>'Operational Data'!I8</f>
         <v>190.84</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="18">
         <v>1299.99</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="0"/>
         <v>989.41666666666663</v>
       </c>
@@ -5655,14 +5667,14 @@
         <f>'Operational Data'!J8</f>
         <v>659.5</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="21">
         <v>1000</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>'Operational Data'!G9</f>
         <v>Prototype Irons</v>
@@ -5678,10 +5690,10 @@
         <f>'Operational Data'!I9</f>
         <v>202.17</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>799.99</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f t="shared" si="0"/>
         <v>484.62</v>
       </c>
@@ -5689,14 +5701,14 @@
         <f>'Operational Data'!J9</f>
         <v>784.5</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <v>1000</v>
       </c>
-      <c r="I9" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I9" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>'Operational Data'!G10</f>
         <v>Standard Irons</v>
@@ -5712,10 +5724,10 @@
         <f>'Operational Data'!I10</f>
         <v>173.76333333333332</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>499.99</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>211.62666666666667</v>
       </c>
@@ -5723,14 +5735,14 @@
         <f>'Operational Data'!J10</f>
         <v>676.83333333333337</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>1000</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>'Operational Data'!G11</f>
         <v>X Forged Irons</v>
@@ -5746,10 +5758,10 @@
         <f>'Operational Data'!I11</f>
         <v>250.34166666666667</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="18">
         <v>599.99</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>236.58166666666671</v>
       </c>
@@ -5757,67 +5769,67 @@
         <f>'Operational Data'!J11</f>
         <v>761.33333333333337</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="21">
         <v>1000</v>
       </c>
-      <c r="I11" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="22"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="22"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="22"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="22"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="22"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="22"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="22"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="I11" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="18"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="18"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5826,12 +5838,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>